<commit_message>
Mac OS support for file names in MongoDB files. gitignore and pipfiles added. Added the XML files to the Git.
</commit_message>
<xml_diff>
--- a/CategoryMapping.xlsx
+++ b/CategoryMapping.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/Desktop/Fallstudie/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/Documents/Repositories/Unicorn_Analytics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC482FC0-70BB-E64F-A5A5-1DE1A71A33CB}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{14491BE0-D4E2-404B-A235-120023C7E78D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="960" windowWidth="27840" windowHeight="16600" xr2:uid="{30B93587-19C8-E44D-8FD2-3737DB33C852}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{30B93587-19C8-E44D-8FD2-3737DB33C852}"/>
   </bookViews>
   <sheets>
     <sheet name="omq_public_categories" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">omq_public_categories!$A$1:$C$1</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -145,13 +148,13 @@
     <t>Startzeiger zeigt immer von Anfang an</t>
   </si>
   <si>
-    <t>category id</t>
-  </si>
-  <si>
-    <t>categoryGroup id</t>
-  </si>
-  <si>
     <t>text</t>
+  </si>
+  <si>
+    <t>category_id</t>
+  </si>
+  <si>
+    <t>categoryGroup_id</t>
   </si>
 </sst>
 </file>
@@ -518,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:C43"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -531,469 +534,474 @@
     <col min="3" max="3" width="169" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>43</v>
+      <c r="A2">
+        <v>125</v>
+      </c>
+      <c r="B2">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>70</v>
+        <v>121</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>71</v>
+        <v>116</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>79</v>
+        <v>112</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>65</v>
+        <v>111</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>85</v>
+        <v>106</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>67</v>
+        <v>99</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="B14">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="B15">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B16">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="B17">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="B18">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="B19">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B20">
         <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B21">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B22">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="B23">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B24">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B25">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
         <v>10</v>
-      </c>
-      <c r="C25" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B26">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="B27">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
         <v>11</v>
-      </c>
-      <c r="C27" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="B28">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B29">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="B30">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="B31">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>104</v>
+        <v>66</v>
       </c>
       <c r="B32">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B33">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="B34">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C34" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="B35">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C35" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>101</v>
+        <v>59</v>
       </c>
       <c r="B36">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C36" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>97</v>
+        <v>57</v>
       </c>
       <c r="B37">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C37" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B38">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C38" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>106</v>
+        <v>55</v>
       </c>
       <c r="B39">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C39" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>112</v>
+        <v>33</v>
       </c>
       <c r="B40">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C40" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="B41">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C41" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>125</v>
+        <v>31</v>
       </c>
       <c r="B42">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C42" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>63</v>
-      </c>
-      <c r="B43">
-        <v>20</v>
-      </c>
-      <c r="C43" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C1" xr:uid="{D7295AB1-C23F-8F41-A0DA-480FE1A6DDDF}">
+    <sortState ref="A2:C42">
+      <sortCondition descending="1" ref="A1:A42"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>